<commit_message>
:bug: chore: God of War III and Watch Dogs 2 links on games.xlsx fixed
</commit_message>
<xml_diff>
--- a/back-end/seeders/games.xlsx
+++ b/back-end/seeders/games.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salva\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\fernando\Documentos\SmartGames\back-end\seeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F7661D-8A78-469A-B5D6-2D671FF10481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714F66B5-04E2-45DE-A7AB-3219665FD460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>PC/PS4/XBoxOne/Switch</t>
-  </si>
-  <si>
-    <t>Loja tambóre/Loja União</t>
   </si>
   <si>
     <t>Spider-Man</t>
@@ -61,9 +58,6 @@
     <t>PS4</t>
   </si>
   <si>
-    <t>Loja tambóre/Loja União/Loja Iguatemi</t>
-  </si>
-  <si>
     <t>God Of War</t>
   </si>
   <si>
@@ -106,9 +100,6 @@
     <t>Kratos está devolta, ainda com a vingança pulsando forte em suas veias. O Olimpo e seus deuses é o seu alvo, não importa o preço que o Deus da Guerra irá pagar. Neste terceiro e épico capítulo você irá controlar Kratos através de batalhas celestiais contra os deuses mais poderosos de todo o Olimpo – inclusive voltará ao inferno e acertar as contas com seu pai colossal e poderoso, Kronos. Deuses como Hermes e Hades não serão páreo para seu poder, os olhos ardentes daquele que busca vingança que nem a mais cruel das mortes pode deter. Enfrente desafios arrasadores e enfrente monstros poderosos como a Quimera, o Cérberus e muitos outros seres místicos que estão ali apenas para acabar com sua existência. Não pare por nada até enfrentar o deus dos deuses: Zeus, e acabar com isso de uma vez por todas.</t>
   </si>
   <si>
-    <t>https://s3.amazonaws.com/comparegame/thumbnails/41421/large.jpg</t>
-  </si>
-  <si>
     <t>PS3/PS4</t>
   </si>
   <si>
@@ -118,9 +109,6 @@
     <t>Junte-se ao Dedsec, um grupo notório de hackers, para executar o maior hack da história; Derrube o ctOS 2.0, um sistema operacional invasivo que está sendo usado por um gênio do crime para monitorar e manipular os cidadãos em uma escala massiva.</t>
   </si>
   <si>
-    <t>https://s3.amazonaws.com/comparegame/thumbnails/42209/large.jpg</t>
-  </si>
-  <si>
     <t>PC/PS4/XBoxOne</t>
   </si>
   <si>
@@ -152,6 +140,18 @@
   </si>
   <si>
     <t>stores</t>
+  </si>
+  <si>
+    <t>Loja Tamboré/Loja União</t>
+  </si>
+  <si>
+    <t>Loja Tamboré/Loja União/Loja Iguatemi</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/a/a9/God_of_War_Logo.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/3/39/WatchDogs2.png</t>
   </si>
 </sst>
 </file>
@@ -346,11 +346,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -403,8 +404,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -720,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,22 +744,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -771,147 +779,147 @@
         <v>3</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="D3" s="4">
         <v>116.9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="D4" s="4">
         <v>69.900000000000006</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="D5" s="4">
         <v>249</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="C6" s="13" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>19</v>
       </c>
       <c r="D6" s="14">
         <v>36</v>
       </c>
       <c r="E6" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="B7" s="12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>24</v>
+      <c r="C7" s="18" t="s">
+        <v>38</v>
       </c>
       <c r="D7" s="14">
         <v>50</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="D8" s="14">
         <v>60</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D9" s="14">
         <v>31</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -921,9 +929,9 @@
     <hyperlink ref="C4" r:id="rId3" xr:uid="{A4991F49-3612-467D-A4F5-ACCBE8FFB2A4}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{2C08E4C8-1A3B-4BF4-9BBD-E53AACCE202C}"/>
     <hyperlink ref="C6" r:id="rId5" xr:uid="{1803C42B-0D84-4121-99B0-0314ABBCEE59}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{E432E3B5-A3A8-4CEA-AF86-EA24F14915A5}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{A81E69BA-1E71-4857-9576-617178C8B074}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{9ADC41D2-7E4A-47A6-8F81-C4951FDB73DB}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{A81E69BA-1E71-4857-9576-617178C8B074}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{9ADC41D2-7E4A-47A6-8F81-C4951FDB73DB}"/>
+    <hyperlink ref="C7" r:id="rId8" xr:uid="{A9990F89-DBF5-457E-9B59-F163931D9FBE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>

</xml_diff>